<commit_message>
Tidied up observed files and ficed figures in apsim simulations
</commit_message>
<xml_diff>
--- a/Prototypes/Canola/Greenethorpe2014.xlsx
+++ b/Prototypes/Canola/Greenethorpe2014.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/lil026_csiro_au/Documents/working/APSIMNextGen/DPAgronomy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{F54E15D8-E584-44AC-BD4F-BA21717B7893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F79CA335-1D96-44E4-82CD-0B26CE861700}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469495C7-88E8-4471-8E6E-FA05F1CD4E12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="3390" windowWidth="21600" windowHeight="11385" xr2:uid="{DCD4BBDB-2039-4016-B509-C04A516B8513}"/>
+    <workbookView xWindow="3570" yWindow="3435" windowWidth="15210" windowHeight="15435" xr2:uid="{DCD4BBDB-2039-4016-B509-C04A516B8513}"/>
   </bookViews>
   <sheets>
-    <sheet name="Obs" sheetId="1" r:id="rId1"/>
+    <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Obs!$B$1:$S$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$B$1:$S$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C11D26-4E0C-495C-A0BC-9CE09D11AC25}">
   <dimension ref="A1:X84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,8 +575,8 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>"Greenethorpe_Ex"&amp;B2&amp;"Cv"&amp;F2</f>
-        <v>Greenethorpe_Ex1CvHyola971_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B2&amp;"Cv"&amp;F2</f>
+        <v>Greenethorpe2014_Ex1CvHyola971_CL</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -585,10 +585,10 @@
         <v>8</v>
       </c>
       <c r="D2" s="1">
-        <v>44270</v>
+        <v>41713</v>
       </c>
       <c r="E2" s="1">
-        <v>44301</v>
+        <v>41744</v>
       </c>
       <c r="F2" t="s">
         <v>26</v>
@@ -640,8 +640,8 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A13" si="0">"Greenethorpe_Ex"&amp;B3&amp;"Cv"&amp;F3</f>
-        <v>Greenethorpe_Ex1CvHyola971_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B3&amp;"Cv"&amp;F3</f>
+        <v>Greenethorpe2014_Ex1CvHyola971_CL</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -650,10 +650,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="1">
-        <v>44270</v>
+        <v>41713</v>
       </c>
       <c r="E3" s="1">
-        <v>44337</v>
+        <v>41780</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
@@ -704,8 +704,8 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f t="shared" si="0"/>
-        <v>Greenethorpe_Ex1CvHyola971_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B4&amp;"Cv"&amp;F4</f>
+        <v>Greenethorpe2014_Ex1CvHyola971_CL</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -714,10 +714,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="1">
-        <v>44270</v>
+        <v>41713</v>
       </c>
       <c r="E4" s="1">
-        <v>44385</v>
+        <v>41828</v>
       </c>
       <c r="F4" t="s">
         <v>26</v>
@@ -768,8 +768,8 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f t="shared" si="0"/>
-        <v>Greenethorpe_Ex1CvHyola971_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B5&amp;"Cv"&amp;F5</f>
+        <v>Greenethorpe2014_Ex1CvHyola971_CL</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -778,10 +778,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="1">
-        <v>44270</v>
+        <v>41713</v>
       </c>
       <c r="E5" s="1">
-        <v>44413</v>
+        <v>41856</v>
       </c>
       <c r="F5" t="s">
         <v>26</v>
@@ -832,8 +832,8 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f t="shared" si="0"/>
-        <v>Greenethorpe_Ex1CvHyola971_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B6&amp;"Cv"&amp;F6</f>
+        <v>Greenethorpe2014_Ex1CvHyola971_CL</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -842,10 +842,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="1">
-        <v>44270</v>
+        <v>41713</v>
       </c>
       <c r="E6" s="1">
-        <v>44442</v>
+        <v>41885</v>
       </c>
       <c r="F6" t="s">
         <v>26</v>
@@ -899,8 +899,8 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f t="shared" si="0"/>
-        <v>Greenethorpe_Ex1CvHyola971_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B7&amp;"Cv"&amp;F7</f>
+        <v>Greenethorpe2014_Ex1CvHyola971_CL</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -909,10 +909,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="1">
-        <v>44270</v>
+        <v>41713</v>
       </c>
       <c r="E7" s="1">
-        <v>44504</v>
+        <v>41947</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -966,8 +966,8 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f t="shared" si="0"/>
-        <v>Greenethorpe_Ex2CvHyola575_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B8&amp;"Cv"&amp;F8</f>
+        <v>Greenethorpe2014_Ex2CvHyola575_CL</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -976,10 +976,10 @@
         <v>8</v>
       </c>
       <c r="D8" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E8" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F8" t="s">
         <v>27</v>
@@ -1030,8 +1030,8 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f t="shared" si="0"/>
-        <v>Greenethorpe_Ex2CvHyola575_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B9&amp;"Cv"&amp;F9</f>
+        <v>Greenethorpe2014_Ex2CvHyola575_CL</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1040,10 +1040,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E9" s="1">
-        <v>44352</v>
+        <v>41795</v>
       </c>
       <c r="F9" t="s">
         <v>27</v>
@@ -1094,8 +1094,8 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f t="shared" si="0"/>
-        <v>Greenethorpe_Ex2CvHyola575_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B10&amp;"Cv"&amp;F10</f>
+        <v>Greenethorpe2014_Ex2CvHyola575_CL</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1104,10 +1104,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E10" s="1">
-        <v>44373</v>
+        <v>41816</v>
       </c>
       <c r="F10" t="s">
         <v>27</v>
@@ -1158,8 +1158,8 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" si="0"/>
-        <v>Greenethorpe_Ex2CvHyola575_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B11&amp;"Cv"&amp;F11</f>
+        <v>Greenethorpe2014_Ex2CvHyola575_CL</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -1168,10 +1168,10 @@
         <v>8</v>
       </c>
       <c r="D11" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E11" s="1">
-        <v>44385</v>
+        <v>41828</v>
       </c>
       <c r="F11" t="s">
         <v>27</v>
@@ -1222,8 +1222,8 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f t="shared" si="0"/>
-        <v>Greenethorpe_Ex2CvHyola575_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B12&amp;"Cv"&amp;F12</f>
+        <v>Greenethorpe2014_Ex2CvHyola575_CL</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -1232,10 +1232,10 @@
         <v>8</v>
       </c>
       <c r="D12" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E12" s="1">
-        <v>44399</v>
+        <v>41842</v>
       </c>
       <c r="F12" t="s">
         <v>27</v>
@@ -1289,8 +1289,8 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" si="0"/>
-        <v>Greenethorpe_Ex2CvHyola575_CL</v>
+        <f>"Greenethorpe2014_Ex"&amp;B13&amp;"Cv"&amp;F13</f>
+        <v>Greenethorpe2014_Ex2CvHyola575_CL</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -1299,10 +1299,10 @@
         <v>8</v>
       </c>
       <c r="D13" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E13" s="1">
-        <v>44490</v>
+        <v>41933</v>
       </c>
       <c r="F13" t="s">
         <v>27</v>
@@ -1356,8 +1356,8 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>"Greenethorpe_Ex"&amp;B14&amp;"Cv"&amp;F14&amp;"TOS"&amp;C14</f>
-        <v>Greenethorpe_Ex3Cv44Y87_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B14&amp;"Cv"&amp;F14&amp;"TOS"&amp;C14</f>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS1</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1366,10 +1366,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E14" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>
@@ -1420,8 +1420,8 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" ref="A15:A73" si="1">"Greenethorpe_Ex"&amp;B15&amp;"Cv"&amp;F15&amp;"TOS"&amp;C15</f>
-        <v>Greenethorpe_Ex3Cv45Y88_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B15&amp;"Cv"&amp;F15&amp;"TOS"&amp;C15</f>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS1</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -1430,10 +1430,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E15" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F15" t="s">
         <v>10</v>
@@ -1484,8 +1484,8 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvATR_GemTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B16&amp;"Cv"&amp;F16&amp;"TOS"&amp;C16</f>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS1</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -1494,10 +1494,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E16" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
@@ -1548,8 +1548,8 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola559_TTTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B17&amp;"Cv"&amp;F17&amp;"TOS"&amp;C17</f>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS1</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -1558,10 +1558,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E17" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
@@ -1612,8 +1612,8 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola575_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B18&amp;"Cv"&amp;F18&amp;"TOS"&amp;C18</f>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS1</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -1622,10 +1622,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E18" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F18" t="s">
         <v>27</v>
@@ -1676,8 +1676,8 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola971_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B19&amp;"Cv"&amp;F19&amp;"TOS"&amp;C19</f>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS1</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -1686,10 +1686,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E19" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F19" t="s">
         <v>26</v>
@@ -1740,8 +1740,8 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola575_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B20&amp;"Cv"&amp;F20&amp;"TOS"&amp;C20</f>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS1</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -1750,10 +1750,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E20" s="1">
-        <v>44364</v>
+        <v>41807</v>
       </c>
       <c r="F20" t="s">
         <v>27</v>
@@ -1807,8 +1807,8 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvATR_GemTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B21&amp;"Cv"&amp;F21&amp;"TOS"&amp;C21</f>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS1</v>
       </c>
       <c r="B21">
         <v>3</v>
@@ -1817,10 +1817,10 @@
         <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E21" s="1">
-        <v>44373</v>
+        <v>41816</v>
       </c>
       <c r="F21" t="s">
         <v>11</v>
@@ -1874,8 +1874,8 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv44Y87_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B22&amp;"Cv"&amp;F22&amp;"TOS"&amp;C22</f>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS1</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1884,10 +1884,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E22" s="1">
-        <v>44393</v>
+        <v>41836</v>
       </c>
       <c r="F22" t="s">
         <v>9</v>
@@ -1941,8 +1941,8 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv45Y88_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B23&amp;"Cv"&amp;F23&amp;"TOS"&amp;C23</f>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS1</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -1951,10 +1951,10 @@
         <v>1</v>
       </c>
       <c r="D23" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E23" s="1">
-        <v>44393</v>
+        <v>41836</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
@@ -2008,8 +2008,8 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola559_TTTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B24&amp;"Cv"&amp;F24&amp;"TOS"&amp;C24</f>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS1</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -2018,10 +2018,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E24" s="1">
-        <v>44393</v>
+        <v>41836</v>
       </c>
       <c r="F24" t="s">
         <v>12</v>
@@ -2075,8 +2075,8 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola971_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B25&amp;"Cv"&amp;F25&amp;"TOS"&amp;C25</f>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS1</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -2085,10 +2085,10 @@
         <v>1</v>
       </c>
       <c r="D25" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E25" s="1">
-        <v>44463</v>
+        <v>41906</v>
       </c>
       <c r="F25" t="s">
         <v>26</v>
@@ -2142,8 +2142,8 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv44Y87_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B26&amp;"Cv"&amp;F26&amp;"TOS"&amp;C26</f>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS1</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -2152,10 +2152,10 @@
         <v>1</v>
       </c>
       <c r="D26" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E26" s="1">
-        <v>44485</v>
+        <v>41928</v>
       </c>
       <c r="F26" t="s">
         <v>9</v>
@@ -2209,8 +2209,8 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv45Y88_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B27&amp;"Cv"&amp;F27&amp;"TOS"&amp;C27</f>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS1</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -2219,10 +2219,10 @@
         <v>1</v>
       </c>
       <c r="D27" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E27" s="1">
-        <v>44485</v>
+        <v>41928</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
@@ -2276,8 +2276,8 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola575_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B28&amp;"Cv"&amp;F28&amp;"TOS"&amp;C28</f>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS1</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -2286,10 +2286,10 @@
         <v>1</v>
       </c>
       <c r="D28" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E28" s="1">
-        <v>44485</v>
+        <v>41928</v>
       </c>
       <c r="F28" t="s">
         <v>27</v>
@@ -2343,8 +2343,8 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvATR_GemTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B29&amp;"Cv"&amp;F29&amp;"TOS"&amp;C29</f>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS1</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -2353,10 +2353,10 @@
         <v>1</v>
       </c>
       <c r="D29" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E29" s="1">
-        <v>44488</v>
+        <v>41931</v>
       </c>
       <c r="F29" t="s">
         <v>11</v>
@@ -2410,8 +2410,8 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola559_TTTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B30&amp;"Cv"&amp;F30&amp;"TOS"&amp;C30</f>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS1</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -2420,10 +2420,10 @@
         <v>1</v>
       </c>
       <c r="D30" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E30" s="1">
-        <v>44490</v>
+        <v>41933</v>
       </c>
       <c r="F30" t="s">
         <v>12</v>
@@ -2477,8 +2477,8 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola971_CLTOS1</v>
+        <f>"Greenethorpe2014_Ex"&amp;B31&amp;"Cv"&amp;F31&amp;"TOS"&amp;C31</f>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS1</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -2487,10 +2487,10 @@
         <v>1</v>
       </c>
       <c r="D31" s="1">
-        <v>44287</v>
+        <v>41730</v>
       </c>
       <c r="E31" s="1">
-        <v>44511</v>
+        <v>41954</v>
       </c>
       <c r="F31" t="s">
         <v>26</v>
@@ -2544,8 +2544,8 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv44Y87_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B32&amp;"Cv"&amp;F32&amp;"TOS"&amp;C32</f>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS2</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -2554,10 +2554,10 @@
         <v>2</v>
       </c>
       <c r="D32" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E32" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F32" t="s">
         <v>9</v>
@@ -2608,8 +2608,8 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv45Y88_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B33&amp;"Cv"&amp;F33&amp;"TOS"&amp;C33</f>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS2</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -2618,10 +2618,10 @@
         <v>2</v>
       </c>
       <c r="D33" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E33" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
@@ -2672,8 +2672,8 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvATR_GemTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B34&amp;"Cv"&amp;F34&amp;"TOS"&amp;C34</f>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS2</v>
       </c>
       <c r="B34">
         <v>3</v>
@@ -2682,10 +2682,10 @@
         <v>2</v>
       </c>
       <c r="D34" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E34" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F34" t="s">
         <v>11</v>
@@ -2736,8 +2736,8 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola559_TTTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B35&amp;"Cv"&amp;F35&amp;"TOS"&amp;C35</f>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS2</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -2746,10 +2746,10 @@
         <v>2</v>
       </c>
       <c r="D35" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E35" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F35" t="s">
         <v>12</v>
@@ -2800,8 +2800,8 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola575_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B36&amp;"Cv"&amp;F36&amp;"TOS"&amp;C36</f>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS2</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -2810,10 +2810,10 @@
         <v>2</v>
       </c>
       <c r="D36" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E36" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F36" t="s">
         <v>27</v>
@@ -2864,8 +2864,8 @@
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola971_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B37&amp;"Cv"&amp;F37&amp;"TOS"&amp;C37</f>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS2</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -2874,10 +2874,10 @@
         <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E37" s="1">
-        <v>44324</v>
+        <v>41767</v>
       </c>
       <c r="F37" t="s">
         <v>26</v>
@@ -2928,8 +2928,8 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvATR_GemTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B38&amp;"Cv"&amp;F38&amp;"TOS"&amp;C38</f>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS2</v>
       </c>
       <c r="B38">
         <v>3</v>
@@ -2938,10 +2938,10 @@
         <v>2</v>
       </c>
       <c r="D38" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E38" s="1">
-        <v>44407</v>
+        <v>41850</v>
       </c>
       <c r="F38" t="s">
         <v>11</v>
@@ -2995,8 +2995,8 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola575_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B39&amp;"Cv"&amp;F39&amp;"TOS"&amp;C39</f>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS2</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -3005,10 +3005,10 @@
         <v>2</v>
       </c>
       <c r="D39" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E39" s="1">
-        <v>44407</v>
+        <v>41850</v>
       </c>
       <c r="F39" t="s">
         <v>27</v>
@@ -3062,8 +3062,8 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv44Y87_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B40&amp;"Cv"&amp;F40&amp;"TOS"&amp;C40</f>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS2</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -3072,10 +3072,10 @@
         <v>2</v>
       </c>
       <c r="D40" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E40" s="1">
-        <v>44414</v>
+        <v>41857</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
@@ -3129,8 +3129,8 @@
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv45Y88_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B41&amp;"Cv"&amp;F41&amp;"TOS"&amp;C41</f>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS2</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -3139,10 +3139,10 @@
         <v>2</v>
       </c>
       <c r="D41" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E41" s="1">
-        <v>44414</v>
+        <v>41857</v>
       </c>
       <c r="F41" t="s">
         <v>10</v>
@@ -3196,8 +3196,8 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola559_TTTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B42&amp;"Cv"&amp;F42&amp;"TOS"&amp;C42</f>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS2</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -3206,10 +3206,10 @@
         <v>2</v>
       </c>
       <c r="D42" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E42" s="1">
-        <v>44414</v>
+        <v>41857</v>
       </c>
       <c r="F42" t="s">
         <v>12</v>
@@ -3263,8 +3263,8 @@
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola971_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B43&amp;"Cv"&amp;F43&amp;"TOS"&amp;C43</f>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS2</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -3273,10 +3273,10 @@
         <v>2</v>
       </c>
       <c r="D43" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E43" s="1">
-        <v>44463</v>
+        <v>41906</v>
       </c>
       <c r="F43" t="s">
         <v>26</v>
@@ -3330,8 +3330,8 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv44Y87_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B44&amp;"Cv"&amp;F44&amp;"TOS"&amp;C44</f>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS2</v>
       </c>
       <c r="B44">
         <v>3</v>
@@ -3340,10 +3340,10 @@
         <v>2</v>
       </c>
       <c r="D44" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E44" s="1">
-        <v>44493</v>
+        <v>41936</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
@@ -3397,8 +3397,8 @@
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv45Y88_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B45&amp;"Cv"&amp;F45&amp;"TOS"&amp;C45</f>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS2</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -3407,10 +3407,10 @@
         <v>2</v>
       </c>
       <c r="D45" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E45" s="1">
-        <v>44493</v>
+        <v>41936</v>
       </c>
       <c r="F45" t="s">
         <v>10</v>
@@ -3464,8 +3464,8 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvATR_GemTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B46&amp;"Cv"&amp;F46&amp;"TOS"&amp;C46</f>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS2</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -3474,10 +3474,10 @@
         <v>2</v>
       </c>
       <c r="D46" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E46" s="1">
-        <v>44493</v>
+        <v>41936</v>
       </c>
       <c r="F46" t="s">
         <v>11</v>
@@ -3531,8 +3531,8 @@
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola559_TTTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B47&amp;"Cv"&amp;F47&amp;"TOS"&amp;C47</f>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS2</v>
       </c>
       <c r="B47">
         <v>3</v>
@@ -3541,10 +3541,10 @@
         <v>2</v>
       </c>
       <c r="D47" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E47" s="1">
-        <v>44493</v>
+        <v>41936</v>
       </c>
       <c r="F47" t="s">
         <v>12</v>
@@ -3598,8 +3598,8 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola575_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B48&amp;"Cv"&amp;F48&amp;"TOS"&amp;C48</f>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS2</v>
       </c>
       <c r="B48">
         <v>3</v>
@@ -3608,10 +3608,10 @@
         <v>2</v>
       </c>
       <c r="D48" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E48" s="1">
-        <v>44493</v>
+        <v>41936</v>
       </c>
       <c r="F48" t="s">
         <v>27</v>
@@ -3665,8 +3665,8 @@
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola971_CLTOS2</v>
+        <f>"Greenethorpe2014_Ex"&amp;B49&amp;"Cv"&amp;F49&amp;"TOS"&amp;C49</f>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS2</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -3675,10 +3675,10 @@
         <v>2</v>
       </c>
       <c r="D49" s="1">
-        <v>44302</v>
+        <v>41745</v>
       </c>
       <c r="E49" s="1">
-        <v>44511</v>
+        <v>41954</v>
       </c>
       <c r="F49" t="s">
         <v>26</v>
@@ -3732,8 +3732,8 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvATR_GemTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B50&amp;"Cv"&amp;F50&amp;"TOS"&amp;C50</f>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS3</v>
       </c>
       <c r="B50">
         <v>3</v>
@@ -3742,10 +3742,10 @@
         <v>3</v>
       </c>
       <c r="D50" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E50" s="1">
-        <v>44420</v>
+        <v>41863</v>
       </c>
       <c r="F50" t="s">
         <v>11</v>
@@ -3799,8 +3799,8 @@
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola575_CLTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B51&amp;"Cv"&amp;F51&amp;"TOS"&amp;C51</f>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS3</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -3809,10 +3809,10 @@
         <v>3</v>
       </c>
       <c r="D51" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E51" s="1">
-        <v>44420</v>
+        <v>41863</v>
       </c>
       <c r="F51" t="s">
         <v>27</v>
@@ -3866,8 +3866,8 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv44Y87_CLTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B52&amp;"Cv"&amp;F52&amp;"TOS"&amp;C52</f>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS3</v>
       </c>
       <c r="B52">
         <v>3</v>
@@ -3876,10 +3876,10 @@
         <v>3</v>
       </c>
       <c r="D52" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E52" s="1">
-        <v>44427</v>
+        <v>41870</v>
       </c>
       <c r="F52" t="s">
         <v>9</v>
@@ -3933,8 +3933,8 @@
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv45Y88_CLTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B53&amp;"Cv"&amp;F53&amp;"TOS"&amp;C53</f>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS3</v>
       </c>
       <c r="B53">
         <v>3</v>
@@ -3943,10 +3943,10 @@
         <v>3</v>
       </c>
       <c r="D53" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E53" s="1">
-        <v>44427</v>
+        <v>41870</v>
       </c>
       <c r="F53" t="s">
         <v>10</v>
@@ -4000,8 +4000,8 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola559_TTTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B54&amp;"Cv"&amp;F54&amp;"TOS"&amp;C54</f>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS3</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -4010,10 +4010,10 @@
         <v>3</v>
       </c>
       <c r="D54" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E54" s="1">
-        <v>44427</v>
+        <v>41870</v>
       </c>
       <c r="F54" t="s">
         <v>12</v>
@@ -4067,8 +4067,8 @@
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola971_CLTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B55&amp;"Cv"&amp;F55&amp;"TOS"&amp;C55</f>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS3</v>
       </c>
       <c r="B55">
         <v>3</v>
@@ -4077,10 +4077,10 @@
         <v>3</v>
       </c>
       <c r="D55" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E55" s="1">
-        <v>44469</v>
+        <v>41912</v>
       </c>
       <c r="F55" t="s">
         <v>26</v>
@@ -4134,8 +4134,8 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv44Y87_CLTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B56&amp;"Cv"&amp;F56&amp;"TOS"&amp;C56</f>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS3</v>
       </c>
       <c r="B56">
         <v>3</v>
@@ -4144,10 +4144,10 @@
         <v>3</v>
       </c>
       <c r="D56" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E56" s="1">
-        <v>44493</v>
+        <v>41936</v>
       </c>
       <c r="F56" t="s">
         <v>9</v>
@@ -4201,8 +4201,8 @@
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv45Y88_CLTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B57&amp;"Cv"&amp;F57&amp;"TOS"&amp;C57</f>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS3</v>
       </c>
       <c r="B57">
         <v>3</v>
@@ -4211,10 +4211,10 @@
         <v>3</v>
       </c>
       <c r="D57" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E57" s="1">
-        <v>44493</v>
+        <v>41936</v>
       </c>
       <c r="F57" t="s">
         <v>10</v>
@@ -4268,8 +4268,8 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvATR_GemTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B58&amp;"Cv"&amp;F58&amp;"TOS"&amp;C58</f>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS3</v>
       </c>
       <c r="B58">
         <v>3</v>
@@ -4278,10 +4278,10 @@
         <v>3</v>
       </c>
       <c r="D58" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E58" s="1">
-        <v>44493</v>
+        <v>41936</v>
       </c>
       <c r="F58" t="s">
         <v>11</v>
@@ -4335,8 +4335,8 @@
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola559_TTTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B59&amp;"Cv"&amp;F59&amp;"TOS"&amp;C59</f>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS3</v>
       </c>
       <c r="B59">
         <v>3</v>
@@ -4345,10 +4345,10 @@
         <v>3</v>
       </c>
       <c r="D59" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E59" s="1">
-        <v>44493</v>
+        <v>41936</v>
       </c>
       <c r="F59" t="s">
         <v>12</v>
@@ -4402,8 +4402,8 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola575_CLTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B60&amp;"Cv"&amp;F60&amp;"TOS"&amp;C60</f>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS3</v>
       </c>
       <c r="B60">
         <v>3</v>
@@ -4412,10 +4412,10 @@
         <v>3</v>
       </c>
       <c r="D60" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E60" s="1">
-        <v>44499</v>
+        <v>41942</v>
       </c>
       <c r="F60" t="s">
         <v>27</v>
@@ -4469,8 +4469,8 @@
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola971_CLTOS3</v>
+        <f>"Greenethorpe2014_Ex"&amp;B61&amp;"Cv"&amp;F61&amp;"TOS"&amp;C61</f>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS3</v>
       </c>
       <c r="B61">
         <v>3</v>
@@ -4479,10 +4479,10 @@
         <v>3</v>
       </c>
       <c r="D61" s="1">
-        <v>44314</v>
+        <v>41757</v>
       </c>
       <c r="E61" s="1">
-        <v>44511</v>
+        <v>41954</v>
       </c>
       <c r="F61" t="s">
         <v>26</v>
@@ -4536,8 +4536,8 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv44Y87_CLTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B62&amp;"Cv"&amp;F62&amp;"TOS"&amp;C62</f>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS4</v>
       </c>
       <c r="B62">
         <v>3</v>
@@ -4546,10 +4546,10 @@
         <v>4</v>
       </c>
       <c r="D62" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E62" s="1">
-        <v>44442</v>
+        <v>41885</v>
       </c>
       <c r="F62" t="s">
         <v>9</v>
@@ -4603,8 +4603,8 @@
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv45Y88_CLTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B63&amp;"Cv"&amp;F63&amp;"TOS"&amp;C63</f>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS4</v>
       </c>
       <c r="B63">
         <v>3</v>
@@ -4613,10 +4613,10 @@
         <v>4</v>
       </c>
       <c r="D63" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E63" s="1">
-        <v>44442</v>
+        <v>41885</v>
       </c>
       <c r="F63" t="s">
         <v>10</v>
@@ -4670,8 +4670,8 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvATR_GemTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B64&amp;"Cv"&amp;F64&amp;"TOS"&amp;C64</f>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS4</v>
       </c>
       <c r="B64">
         <v>3</v>
@@ -4680,10 +4680,10 @@
         <v>4</v>
       </c>
       <c r="D64" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E64" s="1">
-        <v>44442</v>
+        <v>41885</v>
       </c>
       <c r="F64" t="s">
         <v>11</v>
@@ -4737,8 +4737,8 @@
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola559_TTTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B65&amp;"Cv"&amp;F65&amp;"TOS"&amp;C65</f>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS4</v>
       </c>
       <c r="B65">
         <v>3</v>
@@ -4747,10 +4747,10 @@
         <v>4</v>
       </c>
       <c r="D65" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E65" s="1">
-        <v>44442</v>
+        <v>41885</v>
       </c>
       <c r="F65" t="s">
         <v>12</v>
@@ -4804,8 +4804,8 @@
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola575_CLTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B66&amp;"Cv"&amp;F66&amp;"TOS"&amp;C66</f>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS4</v>
       </c>
       <c r="B66">
         <v>3</v>
@@ -4814,10 +4814,10 @@
         <v>4</v>
       </c>
       <c r="D66" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E66" s="1">
-        <v>44442</v>
+        <v>41885</v>
       </c>
       <c r="F66" t="s">
         <v>27</v>
@@ -4871,8 +4871,8 @@
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola971_CLTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B67&amp;"Cv"&amp;F67&amp;"TOS"&amp;C67</f>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS4</v>
       </c>
       <c r="B67">
         <v>3</v>
@@ -4881,10 +4881,10 @@
         <v>4</v>
       </c>
       <c r="D67" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E67" s="1">
-        <v>44476</v>
+        <v>41919</v>
       </c>
       <c r="F67" t="s">
         <v>26</v>
@@ -4938,8 +4938,8 @@
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv44Y87_CLTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B68&amp;"Cv"&amp;F68&amp;"TOS"&amp;C68</f>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS4</v>
       </c>
       <c r="B68">
         <v>3</v>
@@ -4948,10 +4948,10 @@
         <v>4</v>
       </c>
       <c r="D68" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E68" s="1">
-        <v>44493</v>
+        <v>41936</v>
       </c>
       <c r="F68" t="s">
         <v>9</v>
@@ -5005,8 +5005,8 @@
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3Cv45Y88_CLTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B69&amp;"Cv"&amp;F69&amp;"TOS"&amp;C69</f>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS4</v>
       </c>
       <c r="B69">
         <v>3</v>
@@ -5015,10 +5015,10 @@
         <v>4</v>
       </c>
       <c r="D69" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E69" s="1">
-        <v>44499</v>
+        <v>41942</v>
       </c>
       <c r="F69" t="s">
         <v>10</v>
@@ -5072,8 +5072,8 @@
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvATR_GemTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B70&amp;"Cv"&amp;F70&amp;"TOS"&amp;C70</f>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS4</v>
       </c>
       <c r="B70">
         <v>3</v>
@@ -5082,10 +5082,10 @@
         <v>4</v>
       </c>
       <c r="D70" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E70" s="1">
-        <v>44499</v>
+        <v>41942</v>
       </c>
       <c r="F70" t="s">
         <v>11</v>
@@ -5139,8 +5139,8 @@
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola559_TTTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B71&amp;"Cv"&amp;F71&amp;"TOS"&amp;C71</f>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS4</v>
       </c>
       <c r="B71">
         <v>3</v>
@@ -5149,10 +5149,10 @@
         <v>4</v>
       </c>
       <c r="D71" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E71" s="1">
-        <v>44499</v>
+        <v>41942</v>
       </c>
       <c r="F71" t="s">
         <v>12</v>
@@ -5206,8 +5206,8 @@
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola575_CLTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B72&amp;"Cv"&amp;F72&amp;"TOS"&amp;C72</f>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS4</v>
       </c>
       <c r="B72">
         <v>3</v>
@@ -5216,10 +5216,10 @@
         <v>4</v>
       </c>
       <c r="D72" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E72" s="1">
-        <v>44499</v>
+        <v>41942</v>
       </c>
       <c r="F72" t="s">
         <v>27</v>
@@ -5273,8 +5273,8 @@
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f t="shared" si="1"/>
-        <v>Greenethorpe_Ex3CvHyola971_CLTOS4</v>
+        <f>"Greenethorpe2014_Ex"&amp;B73&amp;"Cv"&amp;F73&amp;"TOS"&amp;C73</f>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS4</v>
       </c>
       <c r="B73">
         <v>3</v>
@@ -5283,10 +5283,10 @@
         <v>4</v>
       </c>
       <c r="D73" s="1">
-        <v>44329</v>
+        <v>41772</v>
       </c>
       <c r="E73" s="1">
-        <v>44511</v>
+        <v>41954</v>
       </c>
       <c r="F73" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Added phenology runs and data from Genomics Project
</commit_message>
<xml_diff>
--- a/Prototypes/Canola/Greenethorpe2014.xlsx
+++ b/Prototypes/Canola/Greenethorpe2014.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AA619E12-5329-4A77-AEA6-D19BEBB10224}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC12D7E-2DFB-47E2-921F-129C7F040939}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="24420" windowHeight="13095"/>
+    <workbookView xWindow="4575" yWindow="7590" windowWidth="31770" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="60">
   <si>
     <t>SimulationName</t>
   </si>
@@ -194,12 +194,18 @@
   </si>
   <si>
     <t>Greenethorpe2014_Ex3CvHyola971_CLTOS4</t>
+  </si>
+  <si>
+    <t>Greenethorpe</t>
+  </si>
+  <si>
+    <t>site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1034,3357 +1040,3577 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="5" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>41713</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>41744</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>31</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>60.5</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>65.8</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>9.5</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>41713</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>41780</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>67</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>482.2</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>51.1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>41713</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>41828</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>115</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>39.1</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>699.3</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>6.7</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>219.9</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>41713</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>41856</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>25</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>143</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>38.6</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>635.29999999999995</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>2.7</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>41713</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>41885</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>6</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>172</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>36.200000000000003</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>842.1</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>4.8</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>67.2</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>41713</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>41947</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>25</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>9</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>234</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>28.6</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1057</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>225.1</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0.2</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>3.56</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>63830</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>2761</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>3.3</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>84.7</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>17.7</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>0</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>0.12</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>7004</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>363</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>41745</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>41767</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>28</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>22</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>43.7</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
       <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>41745</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>41795</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>28</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>50</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>58.6</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>129.80000000000001</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>5.7</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>41745</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>41816</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>28</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>71</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>49.6</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>296.3</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>5.0999999999999996</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>34.9</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>41745</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>41828</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>28</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>83</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>52</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>417.4</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>5.8</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>64.5</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>41745</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>41842</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>28</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>6</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>97</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>47.2</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>498.3</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>1.4</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>41745</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>41933</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>28</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>9</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>188</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>45.6</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>1654.2</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>472</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>0.3</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>3.36</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>141552</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>8702</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>3.5</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>88.4</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>27.4</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>0</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>0.09</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>12131</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>552</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14">
         <v>1</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>41730</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>41767</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>31</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>37</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>45.1</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15">
         <v>1</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>41730</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>41767</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>33</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>37</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>48.3</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16">
         <v>1</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>41730</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>41767</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>35</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>37</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>21.4</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17">
         <v>1</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>41730</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>41767</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>37</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>37</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>43.4</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>3.3</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18">
         <v>1</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>41730</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>41767</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>28</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>37</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>46.9</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>3.3</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19">
         <v>1</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>41730</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>41767</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>25</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>37</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>49.8</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>1.8</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>41730</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>41807</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>28</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>6</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>77</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>28</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>481.3</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>5.4</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>16.2</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21">
         <v>1</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>41730</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>41816</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>35</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>6</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>86</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>31.8</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>440.4</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>4.2</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>53.9</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22">
         <v>1</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>41730</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>41836</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>31</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>6</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>106</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>21.6</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>622.4</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>3.4</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23">
         <v>1</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>41730</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>41836</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>33</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>6</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>106</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>27.3</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>670.3</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <v>3.5</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <v>94.9</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24">
         <v>1</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>41730</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>41836</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>37</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>6</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>106</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>27.3</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>507.2</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <v>6.7</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>31.3</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25">
         <v>1</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>41730</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>41906</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>25</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>6</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>176</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>18.399999999999999</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>957.1</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>1.7</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>107.2</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26">
         <v>1</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>41730</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>41928</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>31</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>9</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>198</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>2237</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>685</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>0.8</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>3.83</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>180610</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>10405</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <v>112.1</v>
       </c>
-      <c r="R26">
+      <c r="S26">
         <v>24.9</v>
       </c>
-      <c r="S26">
+      <c r="T26">
         <v>0</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <v>0.22</v>
       </c>
-      <c r="U26">
+      <c r="V26">
         <v>15485</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>289</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27">
         <v>1</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>41730</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>41928</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>33</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>9</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>198</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>2302.9</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>647.79999999999995</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>0.8</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>3.6</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>178696</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>10673</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>234.5</v>
       </c>
-      <c r="R27">
+      <c r="S27">
         <v>96.6</v>
       </c>
-      <c r="S27">
+      <c r="T27">
         <v>0</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <v>0.21</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>18113</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>1255</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28">
         <v>1</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>41730</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>41928</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>28</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>9</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>198</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>2242.6999999999998</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>662.5</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>0.8</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>3.63</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>179234</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>12121</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <v>364.8</v>
       </c>
-      <c r="R28">
+      <c r="S28">
         <v>140.6</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <v>0</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <v>0.21</v>
       </c>
-      <c r="U28">
+      <c r="V28">
         <v>28713</v>
       </c>
-      <c r="V28">
+      <c r="W28">
         <v>2240</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29">
         <v>1</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>41730</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>41931</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>35</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>9</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>201</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>2216.6999999999998</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>739.8</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>0.8</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>3.05</v>
       </c>
-      <c r="N29">
+      <c r="O29">
         <v>247132</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>9165</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <v>226.6</v>
       </c>
-      <c r="R29">
+      <c r="S29">
         <v>99.1</v>
       </c>
-      <c r="S29">
+      <c r="T29">
         <v>0</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <v>0.15</v>
       </c>
-      <c r="U29">
+      <c r="V29">
         <v>46730</v>
       </c>
-      <c r="V29">
+      <c r="W29">
         <v>1036</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30">
         <v>1</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>41730</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>41933</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>37</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>9</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>203</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>2201.3000000000002</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>667.4</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>0.8</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>4</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>168839</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>11985</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>178.3</v>
       </c>
-      <c r="R30">
+      <c r="S30">
         <v>91.8</v>
       </c>
-      <c r="S30">
+      <c r="T30">
         <v>0</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <v>0.13</v>
       </c>
-      <c r="U30">
+      <c r="V30">
         <v>28532</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>1921</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31">
         <v>1</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>41730</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>41954</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>25</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>9</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>224</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>18.399999999999999</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>1276.0999999999999</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>322.89999999999998</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>0.3</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>3.53</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>91425</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>3906</v>
       </c>
-      <c r="P31">
+      <c r="Q31">
         <v>0.8</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <v>43</v>
       </c>
-      <c r="R31">
+      <c r="S31">
         <v>16.100000000000001</v>
       </c>
-      <c r="S31">
+      <c r="T31">
         <v>0</v>
       </c>
-      <c r="T31">
+      <c r="U31">
         <v>0.03</v>
       </c>
-      <c r="U31">
+      <c r="V31">
         <v>3939</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <v>264</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32">
         <v>2</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>41745</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>41767</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>31</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>22</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>48.9</v>
       </c>
-      <c r="P32">
+      <c r="Q32">
         <v>3.6</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33">
         <v>2</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>41745</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <v>41767</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>33</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>22</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>43.4</v>
       </c>
-      <c r="P33">
+      <c r="Q33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34">
         <v>2</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>41745</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <v>41767</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>35</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>22</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>26</v>
       </c>
-      <c r="P34">
+      <c r="Q34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35">
+        <v>58</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35">
         <v>2</v>
       </c>
-      <c r="D35" s="1">
+      <c r="E35" s="1">
         <v>41745</v>
       </c>
-      <c r="E35" s="1">
+      <c r="F35" s="1">
         <v>41767</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>37</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>22</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>45.4</v>
       </c>
-      <c r="P35">
+      <c r="Q35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36">
+        <v>58</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36">
         <v>2</v>
       </c>
-      <c r="D36" s="1">
+      <c r="E36" s="1">
         <v>41745</v>
       </c>
-      <c r="E36" s="1">
+      <c r="F36" s="1">
         <v>41767</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>28</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>22</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>48</v>
       </c>
-      <c r="P36">
+      <c r="Q36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37">
+        <v>58</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37">
         <v>2</v>
       </c>
-      <c r="D37" s="1">
+      <c r="E37" s="1">
         <v>41745</v>
       </c>
-      <c r="E37" s="1">
+      <c r="F37" s="1">
         <v>41767</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>25</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>22</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>45.7</v>
       </c>
-      <c r="P37">
+      <c r="Q37">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38">
+        <v>58</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38">
         <v>2</v>
       </c>
-      <c r="D38" s="1">
+      <c r="E38" s="1">
         <v>41745</v>
       </c>
-      <c r="E38" s="1">
+      <c r="F38" s="1">
         <v>41850</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>35</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>6</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>105</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>43.9</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>542</v>
       </c>
-      <c r="P38">
+      <c r="Q38">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Q38">
+      <c r="R38">
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39">
+        <v>58</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39">
         <v>2</v>
       </c>
-      <c r="D39" s="1">
+      <c r="E39" s="1">
         <v>41745</v>
       </c>
-      <c r="E39" s="1">
+      <c r="F39" s="1">
         <v>41850</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>28</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>6</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>105</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>22.9</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>513.9</v>
       </c>
-      <c r="P39">
+      <c r="Q39">
         <v>1.9</v>
       </c>
-      <c r="Q39">
+      <c r="R39">
         <v>52.8</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40">
+        <v>58</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40">
         <v>2</v>
       </c>
-      <c r="D40" s="1">
+      <c r="E40" s="1">
         <v>41745</v>
       </c>
-      <c r="E40" s="1">
+      <c r="F40" s="1">
         <v>41857</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>31</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>6</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>112</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>44.5</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>764.4</v>
       </c>
-      <c r="P40">
+      <c r="Q40">
         <v>3.9</v>
       </c>
-      <c r="Q40">
+      <c r="R40">
         <v>28.4</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41">
+        <v>58</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41">
         <v>2</v>
       </c>
-      <c r="D41" s="1">
+      <c r="E41" s="1">
         <v>41745</v>
       </c>
-      <c r="E41" s="1">
+      <c r="F41" s="1">
         <v>41857</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>33</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>6</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>112</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>40.700000000000003</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>707.7</v>
       </c>
-      <c r="P41">
+      <c r="Q41">
         <v>0.6</v>
       </c>
-      <c r="Q41">
+      <c r="R41">
         <v>67.5</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C42">
+        <v>58</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42">
         <v>2</v>
       </c>
-      <c r="D42" s="1">
+      <c r="E42" s="1">
         <v>41745</v>
       </c>
-      <c r="E42" s="1">
+      <c r="F42" s="1">
         <v>41857</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>37</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>6</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>112</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>37.5</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>603</v>
       </c>
-      <c r="P42">
+      <c r="Q42">
         <v>5.6</v>
       </c>
-      <c r="Q42">
+      <c r="R42">
         <v>86.1</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
-      </c>
-      <c r="C43">
+        <v>58</v>
+      </c>
+      <c r="C43" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43">
         <v>2</v>
       </c>
-      <c r="D43" s="1">
+      <c r="E43" s="1">
         <v>41745</v>
       </c>
-      <c r="E43" s="1">
+      <c r="F43" s="1">
         <v>41906</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>25</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>6</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>161</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>28</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <v>814.4</v>
       </c>
-      <c r="P43">
+      <c r="Q43">
         <v>4.2</v>
       </c>
-      <c r="Q43">
+      <c r="R43">
         <v>89.7</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44">
+        <v>58</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44">
         <v>2</v>
       </c>
-      <c r="D44" s="1">
+      <c r="E44" s="1">
         <v>41745</v>
       </c>
-      <c r="E44" s="1">
+      <c r="F44" s="1">
         <v>41936</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>31</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>9</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>191</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>1761.8</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>518.5</v>
       </c>
-      <c r="L44">
+      <c r="M44">
         <v>0.3</v>
       </c>
-      <c r="M44">
+      <c r="N44">
         <v>3.69</v>
       </c>
-      <c r="N44">
+      <c r="O44">
         <v>140510</v>
       </c>
-      <c r="O44">
+      <c r="P44">
         <v>7231</v>
       </c>
-      <c r="Q44">
+      <c r="R44">
         <v>47.2</v>
       </c>
-      <c r="R44">
+      <c r="S44">
         <v>9.1</v>
       </c>
-      <c r="S44">
+      <c r="T44">
         <v>0</v>
       </c>
-      <c r="T44">
+      <c r="U44">
         <v>0.02</v>
       </c>
-      <c r="U44">
+      <c r="V44">
         <v>3291</v>
       </c>
-      <c r="V44">
+      <c r="W44">
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>30</v>
-      </c>
-      <c r="C45">
+        <v>58</v>
+      </c>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45">
         <v>2</v>
       </c>
-      <c r="D45" s="1">
+      <c r="E45" s="1">
         <v>41745</v>
       </c>
-      <c r="E45" s="1">
+      <c r="F45" s="1">
         <v>41936</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>33</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>9</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>191</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <v>1718.5</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>506.4</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <v>0.3</v>
       </c>
-      <c r="M45">
+      <c r="N45">
         <v>3.65</v>
       </c>
-      <c r="N45">
+      <c r="O45">
         <v>139424</v>
       </c>
-      <c r="O45">
+      <c r="P45">
         <v>7657</v>
       </c>
-      <c r="Q45">
+      <c r="R45">
         <v>136.1</v>
       </c>
-      <c r="R45">
+      <c r="S45">
         <v>31.9</v>
       </c>
-      <c r="S45">
+      <c r="T45">
         <v>0</v>
       </c>
-      <c r="T45">
+      <c r="U45">
         <v>0.11</v>
       </c>
-      <c r="U45">
+      <c r="V45">
         <v>12050</v>
       </c>
-      <c r="V45">
+      <c r="W45">
         <v>688</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46">
+        <v>58</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46">
         <v>2</v>
       </c>
-      <c r="D46" s="1">
+      <c r="E46" s="1">
         <v>41745</v>
       </c>
-      <c r="E46" s="1">
+      <c r="F46" s="1">
         <v>41936</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>35</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>9</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>191</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <v>1373.4</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>441.9</v>
       </c>
-      <c r="L46">
+      <c r="M46">
         <v>0.3</v>
       </c>
-      <c r="M46">
+      <c r="N46">
         <v>3.44</v>
       </c>
-      <c r="N46">
+      <c r="O46">
         <v>129123</v>
       </c>
-      <c r="O46">
+      <c r="P46">
         <v>4898</v>
       </c>
-      <c r="Q46">
+      <c r="R46">
         <v>37.4</v>
       </c>
-      <c r="R46">
+      <c r="S46">
         <v>13.6</v>
       </c>
-      <c r="S46">
+      <c r="T46">
         <v>0</v>
       </c>
-      <c r="T46">
+      <c r="U46">
         <v>0.18</v>
       </c>
-      <c r="U46">
+      <c r="V46">
         <v>7997</v>
       </c>
-      <c r="V46">
+      <c r="W46">
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47">
+        <v>58</v>
+      </c>
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47">
         <v>2</v>
       </c>
-      <c r="D47" s="1">
+      <c r="E47" s="1">
         <v>41745</v>
       </c>
-      <c r="E47" s="1">
+      <c r="F47" s="1">
         <v>41936</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>37</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>9</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>191</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <v>1487.7</v>
       </c>
-      <c r="K47">
+      <c r="L47">
         <v>484.5</v>
       </c>
-      <c r="L47">
+      <c r="M47">
         <v>0.3</v>
       </c>
-      <c r="M47">
+      <c r="N47">
         <v>3.65</v>
       </c>
-      <c r="N47">
+      <c r="O47">
         <v>133383</v>
       </c>
-      <c r="O47">
+      <c r="P47">
         <v>6821</v>
       </c>
-      <c r="Q47">
+      <c r="R47">
         <v>70.599999999999994</v>
       </c>
-      <c r="R47">
+      <c r="S47">
         <v>23.2</v>
       </c>
-      <c r="S47">
+      <c r="T47">
         <v>0</v>
       </c>
-      <c r="T47">
+      <c r="U47">
         <v>0.16</v>
       </c>
-      <c r="U47">
+      <c r="V47">
         <v>9262</v>
       </c>
-      <c r="V47">
+      <c r="W47">
         <v>648</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>30</v>
-      </c>
-      <c r="C48">
+        <v>58</v>
+      </c>
+      <c r="C48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48">
         <v>2</v>
       </c>
-      <c r="D48" s="1">
+      <c r="E48" s="1">
         <v>41745</v>
       </c>
-      <c r="E48" s="1">
+      <c r="F48" s="1">
         <v>41936</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>28</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>9</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>191</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>1887.5</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>540.9</v>
       </c>
-      <c r="L48">
+      <c r="M48">
         <v>0.3</v>
       </c>
-      <c r="M48">
+      <c r="N48">
         <v>3.44</v>
       </c>
-      <c r="N48">
+      <c r="O48">
         <v>157307</v>
       </c>
-      <c r="O48">
+      <c r="P48">
         <v>9749</v>
       </c>
-      <c r="Q48">
+      <c r="R48">
         <v>51.6</v>
       </c>
-      <c r="R48">
+      <c r="S48">
         <v>23</v>
       </c>
-      <c r="S48">
+      <c r="T48">
         <v>0</v>
       </c>
-      <c r="T48">
+      <c r="U48">
         <v>0.05</v>
       </c>
-      <c r="U48">
+      <c r="V48">
         <v>8263</v>
       </c>
-      <c r="V48">
+      <c r="W48">
         <v>300</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49">
+        <v>58</v>
+      </c>
+      <c r="C49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49">
         <v>2</v>
       </c>
-      <c r="D49" s="1">
+      <c r="E49" s="1">
         <v>41745</v>
       </c>
-      <c r="E49" s="1">
+      <c r="F49" s="1">
         <v>41954</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>25</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>9</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>209</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>24.5</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <v>1191.7</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>284.5</v>
       </c>
-      <c r="L49">
+      <c r="M49">
         <v>0.2</v>
       </c>
-      <c r="M49">
+      <c r="N49">
         <v>3.58</v>
       </c>
-      <c r="N49">
+      <c r="O49">
         <v>79634</v>
       </c>
-      <c r="O49">
+      <c r="P49">
         <v>3413</v>
       </c>
-      <c r="P49">
+      <c r="Q49">
         <v>2.8</v>
       </c>
-      <c r="Q49">
+      <c r="R49">
         <v>42.7</v>
       </c>
-      <c r="R49">
+      <c r="S49">
         <v>20.9</v>
       </c>
-      <c r="S49">
+      <c r="T49">
         <v>0</v>
       </c>
-      <c r="T49">
+      <c r="U49">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="U49">
+      <c r="V49">
         <v>6778</v>
       </c>
-      <c r="V49">
+      <c r="W49">
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>46</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
-      </c>
-      <c r="C50">
+        <v>58</v>
+      </c>
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50">
         <v>3</v>
       </c>
-      <c r="D50" s="1">
+      <c r="E50" s="1">
         <v>41757</v>
       </c>
-      <c r="E50" s="1">
+      <c r="F50" s="1">
         <v>41863</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>35</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>6</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>106</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>36.9</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <v>392.3</v>
       </c>
-      <c r="P50">
+      <c r="Q50">
         <v>4.4000000000000004</v>
       </c>
-      <c r="Q50">
+      <c r="R50">
         <v>24.2</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51">
+        <v>58</v>
+      </c>
+      <c r="C51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51">
         <v>3</v>
       </c>
-      <c r="D51" s="1">
+      <c r="E51" s="1">
         <v>41757</v>
       </c>
-      <c r="E51" s="1">
+      <c r="F51" s="1">
         <v>41863</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>28</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>6</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>106</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>36.200000000000003</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <v>589.70000000000005</v>
       </c>
-      <c r="P51">
+      <c r="Q51">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Q51">
+      <c r="R51">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>30</v>
-      </c>
-      <c r="C52">
+        <v>58</v>
+      </c>
+      <c r="C52" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52">
         <v>3</v>
       </c>
-      <c r="D52" s="1">
+      <c r="E52" s="1">
         <v>41757</v>
       </c>
-      <c r="E52" s="1">
+      <c r="F52" s="1">
         <v>41870</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>31</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>6</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>113</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>38.1</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>737.4</v>
       </c>
-      <c r="P52">
+      <c r="Q52">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q52">
+      <c r="R52">
         <v>84.9</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>49</v>
       </c>
       <c r="B53" t="s">
-        <v>30</v>
-      </c>
-      <c r="C53">
+        <v>58</v>
+      </c>
+      <c r="C53" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53">
         <v>3</v>
       </c>
-      <c r="D53" s="1">
+      <c r="E53" s="1">
         <v>41757</v>
       </c>
-      <c r="E53" s="1">
+      <c r="F53" s="1">
         <v>41870</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>33</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>6</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>113</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>34.299999999999997</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <v>763.4</v>
       </c>
-      <c r="P53">
+      <c r="Q53">
         <v>7.2</v>
       </c>
-      <c r="Q53">
+      <c r="R53">
         <v>170.7</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>50</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
-      </c>
-      <c r="C54">
+        <v>58</v>
+      </c>
+      <c r="C54" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54">
         <v>3</v>
       </c>
-      <c r="D54" s="1">
+      <c r="E54" s="1">
         <v>41757</v>
       </c>
-      <c r="E54" s="1">
+      <c r="F54" s="1">
         <v>41870</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>37</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>6</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <v>113</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>33.1</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <v>642.70000000000005</v>
       </c>
-      <c r="P54">
+      <c r="Q54">
         <v>5.4</v>
       </c>
-      <c r="Q54">
+      <c r="R54">
         <v>57</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55">
+        <v>58</v>
+      </c>
+      <c r="C55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55">
         <v>3</v>
       </c>
-      <c r="D55" s="1">
+      <c r="E55" s="1">
         <v>41757</v>
       </c>
-      <c r="E55" s="1">
+      <c r="F55" s="1">
         <v>41912</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>25</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>6</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>155</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>33.1</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>1048.3</v>
       </c>
-      <c r="P55">
+      <c r="Q55">
         <v>2.5</v>
       </c>
-      <c r="Q55">
+      <c r="R55">
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>48</v>
       </c>
       <c r="B56" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56">
+        <v>58</v>
+      </c>
+      <c r="C56" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56">
         <v>3</v>
       </c>
-      <c r="D56" s="1">
+      <c r="E56" s="1">
         <v>41757</v>
       </c>
-      <c r="E56" s="1">
+      <c r="F56" s="1">
         <v>41936</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>31</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>9</v>
       </c>
-      <c r="H56">
+      <c r="I56">
         <v>179</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <v>1599.9</v>
       </c>
-      <c r="K56">
+      <c r="L56">
         <v>456</v>
       </c>
-      <c r="L56">
+      <c r="M56">
         <v>0.3</v>
       </c>
-      <c r="M56">
+      <c r="N56">
         <v>3.52</v>
       </c>
-      <c r="N56">
+      <c r="O56">
         <v>130120</v>
       </c>
-      <c r="O56">
+      <c r="P56">
         <v>6889</v>
       </c>
-      <c r="Q56">
+      <c r="R56">
         <v>65.7</v>
       </c>
-      <c r="R56">
+      <c r="S56">
         <v>11.9</v>
       </c>
-      <c r="S56">
+      <c r="T56">
         <v>0</v>
       </c>
-      <c r="T56">
+      <c r="U56">
         <v>0.18</v>
       </c>
-      <c r="U56">
+      <c r="V56">
         <v>5744</v>
       </c>
-      <c r="V56">
+      <c r="W56">
         <v>300</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>49</v>
       </c>
       <c r="B57" t="s">
-        <v>30</v>
-      </c>
-      <c r="C57">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57">
         <v>3</v>
       </c>
-      <c r="D57" s="1">
+      <c r="E57" s="1">
         <v>41757</v>
       </c>
-      <c r="E57" s="1">
+      <c r="F57" s="1">
         <v>41936</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>33</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>9</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>179</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <v>1694.9</v>
       </c>
-      <c r="K57">
+      <c r="L57">
         <v>468.9</v>
       </c>
-      <c r="L57">
+      <c r="M57">
         <v>0.3</v>
       </c>
-      <c r="M57">
+      <c r="N57">
         <v>3.28</v>
       </c>
-      <c r="N57">
+      <c r="O57">
         <v>142900</v>
       </c>
-      <c r="O57">
+      <c r="P57">
         <v>7237</v>
       </c>
-      <c r="Q57">
+      <c r="R57">
         <v>77.8</v>
       </c>
-      <c r="R57">
+      <c r="S57">
         <v>19</v>
       </c>
-      <c r="S57">
+      <c r="T57">
         <v>0</v>
       </c>
-      <c r="T57">
+      <c r="U57">
         <v>0.11</v>
       </c>
-      <c r="U57">
+      <c r="V57">
         <v>4813</v>
       </c>
-      <c r="V57">
+      <c r="W57">
         <v>456</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>30</v>
-      </c>
-      <c r="C58">
+        <v>58</v>
+      </c>
+      <c r="C58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58">
         <v>3</v>
       </c>
-      <c r="D58" s="1">
+      <c r="E58" s="1">
         <v>41757</v>
       </c>
-      <c r="E58" s="1">
+      <c r="F58" s="1">
         <v>41936</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>35</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>9</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <v>179</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <v>1285</v>
       </c>
-      <c r="K58">
+      <c r="L58">
         <v>386.4</v>
       </c>
-      <c r="L58">
+      <c r="M58">
         <v>0.3</v>
       </c>
-      <c r="M58">
+      <c r="N58">
         <v>3.17</v>
       </c>
-      <c r="N58">
+      <c r="O58">
         <v>122939</v>
       </c>
-      <c r="O58">
+      <c r="P58">
         <v>5193</v>
       </c>
-      <c r="Q58">
+      <c r="R58">
         <v>38.9</v>
       </c>
-      <c r="R58">
+      <c r="S58">
         <v>17.8</v>
       </c>
-      <c r="S58">
+      <c r="T58">
         <v>0</v>
       </c>
-      <c r="T58">
+      <c r="U58">
         <v>0.17</v>
       </c>
-      <c r="U58">
+      <c r="V58">
         <v>11857</v>
       </c>
-      <c r="V58">
+      <c r="W58">
         <v>254</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>30</v>
-      </c>
-      <c r="C59">
+        <v>58</v>
+      </c>
+      <c r="C59" t="s">
+        <v>30</v>
+      </c>
+      <c r="D59">
         <v>3</v>
       </c>
-      <c r="D59" s="1">
+      <c r="E59" s="1">
         <v>41757</v>
       </c>
-      <c r="E59" s="1">
+      <c r="F59" s="1">
         <v>41936</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>37</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>9</v>
       </c>
-      <c r="H59">
+      <c r="I59">
         <v>179</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <v>1545.6</v>
       </c>
-      <c r="K59">
+      <c r="L59">
         <v>494.2</v>
       </c>
-      <c r="L59">
+      <c r="M59">
         <v>0.3</v>
       </c>
-      <c r="M59">
+      <c r="N59">
         <v>3.53</v>
       </c>
-      <c r="N59">
+      <c r="O59">
         <v>140012</v>
       </c>
-      <c r="O59">
+      <c r="P59">
         <v>7716</v>
       </c>
-      <c r="Q59">
+      <c r="R59">
         <v>141.1</v>
       </c>
-      <c r="R59">
+      <c r="S59">
         <v>49.9</v>
-      </c>
-      <c r="S59">
-        <v>0</v>
       </c>
       <c r="T59">
         <v>0</v>
       </c>
       <c r="U59">
+        <v>0</v>
+      </c>
+      <c r="V59">
         <v>13982</v>
       </c>
-      <c r="V59">
+      <c r="W59">
         <v>1282</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>47</v>
       </c>
       <c r="B60" t="s">
-        <v>30</v>
-      </c>
-      <c r="C60">
+        <v>58</v>
+      </c>
+      <c r="C60" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60">
         <v>3</v>
       </c>
-      <c r="D60" s="1">
+      <c r="E60" s="1">
         <v>41757</v>
       </c>
-      <c r="E60" s="1">
+      <c r="F60" s="1">
         <v>41942</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>28</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>9</v>
       </c>
-      <c r="H60">
+      <c r="I60">
         <v>185</v>
       </c>
-      <c r="J60">
+      <c r="K60">
         <v>1683.5</v>
       </c>
-      <c r="K60">
+      <c r="L60">
         <v>406.6</v>
       </c>
-      <c r="L60">
+      <c r="M60">
         <v>0.2</v>
       </c>
-      <c r="M60">
+      <c r="N60">
         <v>2.86</v>
       </c>
-      <c r="N60">
+      <c r="O60">
         <v>143517</v>
       </c>
-      <c r="O60">
+      <c r="P60">
         <v>8183</v>
       </c>
-      <c r="Q60">
+      <c r="R60">
         <v>8.1999999999999993</v>
       </c>
-      <c r="R60">
+      <c r="S60">
         <v>8.5</v>
       </c>
-      <c r="S60">
+      <c r="T60">
         <v>0</v>
       </c>
-      <c r="T60">
+      <c r="U60">
         <v>0.21</v>
       </c>
-      <c r="U60">
+      <c r="V60">
         <v>7764</v>
       </c>
-      <c r="V60">
+      <c r="W60">
         <v>381</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>51</v>
       </c>
       <c r="B61" t="s">
-        <v>30</v>
-      </c>
-      <c r="C61">
+        <v>58</v>
+      </c>
+      <c r="C61" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61">
         <v>3</v>
       </c>
-      <c r="D61" s="1">
+      <c r="E61" s="1">
         <v>41757</v>
       </c>
-      <c r="E61" s="1">
+      <c r="F61" s="1">
         <v>41954</v>
       </c>
-      <c r="F61" t="s">
+      <c r="G61" t="s">
         <v>25</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>9</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <v>197</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>22.3</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <v>885.5</v>
       </c>
-      <c r="K61">
+      <c r="L61">
         <v>190</v>
       </c>
-      <c r="L61">
+      <c r="M61">
         <v>0.2</v>
       </c>
-      <c r="M61">
+      <c r="N61">
         <v>3.25</v>
       </c>
-      <c r="N61">
+      <c r="O61">
         <v>58772</v>
       </c>
-      <c r="O61">
+      <c r="P61">
         <v>3053</v>
       </c>
-      <c r="P61">
+      <c r="Q61">
         <v>1.9</v>
       </c>
-      <c r="Q61">
+      <c r="R61">
         <v>51.4</v>
       </c>
-      <c r="R61">
+      <c r="S61">
         <v>16.3</v>
       </c>
-      <c r="S61">
+      <c r="T61">
         <v>0</v>
       </c>
-      <c r="T61">
+      <c r="U61">
         <v>0.13</v>
       </c>
-      <c r="U61">
+      <c r="V61">
         <v>6458</v>
       </c>
-      <c r="V61">
+      <c r="W61">
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>52</v>
       </c>
       <c r="B62" t="s">
-        <v>30</v>
-      </c>
-      <c r="C62">
+        <v>58</v>
+      </c>
+      <c r="C62" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62">
         <v>4</v>
       </c>
-      <c r="D62" s="1">
+      <c r="E62" s="1">
         <v>41772</v>
       </c>
-      <c r="E62" s="1">
+      <c r="F62" s="1">
         <v>41885</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>31</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>6</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <v>113</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <v>31.8</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>516.79999999999995</v>
       </c>
-      <c r="P62">
+      <c r="Q62">
         <v>4.5999999999999996</v>
       </c>
-      <c r="Q62">
+      <c r="R62">
         <v>69.3</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>53</v>
       </c>
       <c r="B63" t="s">
-        <v>30</v>
-      </c>
-      <c r="C63">
+        <v>58</v>
+      </c>
+      <c r="C63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63">
         <v>4</v>
       </c>
-      <c r="D63" s="1">
+      <c r="E63" s="1">
         <v>41772</v>
       </c>
-      <c r="E63" s="1">
+      <c r="F63" s="1">
         <v>41885</v>
       </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>33</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>6</v>
       </c>
-      <c r="H63">
+      <c r="I63">
         <v>113</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>30.5</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <v>592.9</v>
       </c>
-      <c r="P63">
+      <c r="Q63">
         <v>4</v>
       </c>
-      <c r="Q63">
+      <c r="R63">
         <v>60.9</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>54</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
-      </c>
-      <c r="C64">
+        <v>58</v>
+      </c>
+      <c r="C64" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64">
         <v>4</v>
       </c>
-      <c r="D64" s="1">
+      <c r="E64" s="1">
         <v>41772</v>
       </c>
-      <c r="E64" s="1">
+      <c r="F64" s="1">
         <v>41885</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>35</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>6</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>113</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>45.8</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>482.4</v>
       </c>
-      <c r="P64">
+      <c r="Q64">
         <v>7.6</v>
       </c>
-      <c r="Q64">
+      <c r="R64">
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>30</v>
-      </c>
-      <c r="C65">
+        <v>58</v>
+      </c>
+      <c r="C65" t="s">
+        <v>30</v>
+      </c>
+      <c r="D65">
         <v>4</v>
       </c>
-      <c r="D65" s="1">
+      <c r="E65" s="1">
         <v>41772</v>
       </c>
-      <c r="E65" s="1">
+      <c r="F65" s="1">
         <v>41885</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>37</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>6</v>
       </c>
-      <c r="H65">
+      <c r="I65">
         <v>113</v>
       </c>
-      <c r="I65">
+      <c r="J65">
         <v>33.1</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <v>440.2</v>
       </c>
-      <c r="P65">
+      <c r="Q65">
         <v>1.7</v>
       </c>
-      <c r="Q65">
+      <c r="R65">
         <v>17.3</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>30</v>
-      </c>
-      <c r="C66">
+        <v>58</v>
+      </c>
+      <c r="C66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66">
         <v>4</v>
       </c>
-      <c r="D66" s="1">
+      <c r="E66" s="1">
         <v>41772</v>
       </c>
-      <c r="E66" s="1">
+      <c r="F66" s="1">
         <v>41885</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>28</v>
       </c>
-      <c r="G66">
+      <c r="H66">
         <v>6</v>
       </c>
-      <c r="H66">
+      <c r="I66">
         <v>113</v>
       </c>
-      <c r="I66">
+      <c r="J66">
         <v>40.700000000000003</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <v>569.79999999999995</v>
       </c>
-      <c r="P66">
+      <c r="Q66">
         <v>0.6</v>
       </c>
-      <c r="Q66">
+      <c r="R66">
         <v>47.3</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>57</v>
       </c>
       <c r="B67" t="s">
-        <v>30</v>
-      </c>
-      <c r="C67">
+        <v>58</v>
+      </c>
+      <c r="C67" t="s">
+        <v>30</v>
+      </c>
+      <c r="D67">
         <v>4</v>
       </c>
-      <c r="D67" s="1">
+      <c r="E67" s="1">
         <v>41772</v>
       </c>
-      <c r="E67" s="1">
+      <c r="F67" s="1">
         <v>41919</v>
       </c>
-      <c r="F67" t="s">
+      <c r="G67" t="s">
         <v>25</v>
       </c>
-      <c r="G67">
+      <c r="H67">
         <v>6</v>
       </c>
-      <c r="H67">
+      <c r="I67">
         <v>147</v>
       </c>
-      <c r="I67">
+      <c r="J67">
         <v>36.200000000000003</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>606.9</v>
       </c>
-      <c r="P67">
+      <c r="Q67">
         <v>4.4000000000000004</v>
       </c>
-      <c r="Q67">
+      <c r="R67">
         <v>26.8</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>52</v>
       </c>
       <c r="B68" t="s">
-        <v>30</v>
-      </c>
-      <c r="C68">
+        <v>58</v>
+      </c>
+      <c r="C68" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68">
         <v>4</v>
       </c>
-      <c r="D68" s="1">
+      <c r="E68" s="1">
         <v>41772</v>
       </c>
-      <c r="E68" s="1">
+      <c r="F68" s="1">
         <v>41936</v>
       </c>
-      <c r="F68" t="s">
+      <c r="G68" t="s">
         <v>31</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>9</v>
       </c>
-      <c r="H68">
+      <c r="I68">
         <v>164</v>
       </c>
-      <c r="J68">
+      <c r="K68">
         <v>1303.7</v>
       </c>
-      <c r="K68">
+      <c r="L68">
         <v>365.4</v>
       </c>
-      <c r="L68">
+      <c r="M68">
         <v>0.3</v>
       </c>
-      <c r="M68">
+      <c r="N68">
         <v>3.23</v>
       </c>
-      <c r="N68">
+      <c r="O68">
         <v>113082</v>
       </c>
-      <c r="O68">
+      <c r="P68">
         <v>5575</v>
       </c>
-      <c r="Q68">
+      <c r="R68">
         <v>62.4</v>
       </c>
-      <c r="R68">
+      <c r="S68">
         <v>18.100000000000001</v>
       </c>
-      <c r="S68">
+      <c r="T68">
         <v>0</v>
       </c>
-      <c r="T68">
+      <c r="U68">
         <v>0.03</v>
       </c>
-      <c r="U68">
+      <c r="V68">
         <v>4546</v>
       </c>
-      <c r="V68">
+      <c r="W68">
         <v>284</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>53</v>
       </c>
       <c r="B69" t="s">
-        <v>30</v>
-      </c>
-      <c r="C69">
+        <v>58</v>
+      </c>
+      <c r="C69" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69">
         <v>4</v>
       </c>
-      <c r="D69" s="1">
+      <c r="E69" s="1">
         <v>41772</v>
       </c>
-      <c r="E69" s="1">
+      <c r="F69" s="1">
         <v>41942</v>
       </c>
-      <c r="F69" t="s">
+      <c r="G69" t="s">
         <v>33</v>
       </c>
-      <c r="G69">
+      <c r="H69">
         <v>9</v>
       </c>
-      <c r="H69">
+      <c r="I69">
         <v>170</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <v>10.5</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>1400.1</v>
       </c>
-      <c r="K69">
+      <c r="L69">
         <v>379.8</v>
       </c>
-      <c r="L69">
+      <c r="M69">
         <v>0.3</v>
       </c>
-      <c r="M69">
+      <c r="N69">
         <v>2.91</v>
       </c>
-      <c r="N69">
+      <c r="O69">
         <v>129658</v>
       </c>
-      <c r="O69">
+      <c r="P69">
         <v>6392</v>
       </c>
-      <c r="Q69">
+      <c r="R69">
         <v>134.9</v>
       </c>
-      <c r="R69">
+      <c r="S69">
         <v>40</v>
       </c>
-      <c r="S69">
+      <c r="T69">
         <v>0</v>
       </c>
-      <c r="T69">
+      <c r="U69">
         <v>0.14000000000000001</v>
       </c>
-      <c r="U69">
+      <c r="V69">
         <v>7713</v>
       </c>
-      <c r="V69">
+      <c r="W69">
         <v>429</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>54</v>
       </c>
       <c r="B70" t="s">
-        <v>30</v>
-      </c>
-      <c r="C70">
+        <v>58</v>
+      </c>
+      <c r="C70" t="s">
+        <v>30</v>
+      </c>
+      <c r="D70">
         <v>4</v>
       </c>
-      <c r="D70" s="1">
+      <c r="E70" s="1">
         <v>41772</v>
       </c>
-      <c r="E70" s="1">
+      <c r="F70" s="1">
         <v>41942</v>
       </c>
-      <c r="F70" t="s">
+      <c r="G70" t="s">
         <v>35</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>9</v>
       </c>
-      <c r="H70">
+      <c r="I70">
         <v>170</v>
       </c>
-      <c r="I70">
+      <c r="J70">
         <v>43.4</v>
       </c>
-      <c r="J70">
+      <c r="K70">
         <v>1067.2</v>
       </c>
-      <c r="K70">
+      <c r="L70">
         <v>291.60000000000002</v>
       </c>
-      <c r="L70">
+      <c r="M70">
         <v>0.3</v>
       </c>
-      <c r="M70">
+      <c r="N70">
         <v>2.9</v>
       </c>
-      <c r="N70">
+      <c r="O70">
         <v>100533</v>
       </c>
-      <c r="O70">
+      <c r="P70">
         <v>3699</v>
       </c>
-      <c r="P70">
+      <c r="Q70">
         <v>2.4</v>
       </c>
-      <c r="Q70">
+      <c r="R70">
         <v>80.099999999999994</v>
       </c>
-      <c r="R70">
+      <c r="S70">
         <v>12.1</v>
       </c>
-      <c r="S70">
+      <c r="T70">
         <v>0</v>
       </c>
-      <c r="T70">
+      <c r="U70">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="U70">
+      <c r="V70">
         <v>2772</v>
       </c>
-      <c r="V70">
+      <c r="W70">
         <v>340</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>55</v>
       </c>
       <c r="B71" t="s">
-        <v>30</v>
-      </c>
-      <c r="C71">
+        <v>58</v>
+      </c>
+      <c r="C71" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71">
         <v>4</v>
       </c>
-      <c r="D71" s="1">
+      <c r="E71" s="1">
         <v>41772</v>
       </c>
-      <c r="E71" s="1">
+      <c r="F71" s="1">
         <v>41942</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>37</v>
       </c>
-      <c r="G71">
+      <c r="H71">
         <v>9</v>
       </c>
-      <c r="H71">
+      <c r="I71">
         <v>170</v>
       </c>
-      <c r="I71">
+      <c r="J71">
         <v>30.9</v>
       </c>
-      <c r="J71">
+      <c r="K71">
         <v>1045.8</v>
       </c>
-      <c r="K71">
+      <c r="L71">
         <v>314.3</v>
       </c>
-      <c r="L71">
+      <c r="M71">
         <v>0.3</v>
       </c>
-      <c r="M71">
+      <c r="N71">
         <v>2.99</v>
       </c>
-      <c r="N71">
+      <c r="O71">
         <v>104800</v>
       </c>
-      <c r="O71">
+      <c r="P71">
         <v>5200</v>
       </c>
-      <c r="P71">
+      <c r="Q71">
         <v>1.9</v>
       </c>
-      <c r="Q71">
+      <c r="R71">
         <v>108.9</v>
       </c>
-      <c r="R71">
+      <c r="S71">
         <v>33.700000000000003</v>
       </c>
-      <c r="S71">
+      <c r="T71">
         <v>0</v>
       </c>
-      <c r="T71">
+      <c r="U71">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="U71">
+      <c r="V71">
         <v>8921</v>
       </c>
-      <c r="V71">
+      <c r="W71">
         <v>231</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>56</v>
       </c>
       <c r="B72" t="s">
-        <v>30</v>
-      </c>
-      <c r="C72">
+        <v>58</v>
+      </c>
+      <c r="C72" t="s">
+        <v>30</v>
+      </c>
+      <c r="D72">
         <v>4</v>
       </c>
-      <c r="D72" s="1">
+      <c r="E72" s="1">
         <v>41772</v>
       </c>
-      <c r="E72" s="1">
+      <c r="F72" s="1">
         <v>41942</v>
       </c>
-      <c r="F72" t="s">
+      <c r="G72" t="s">
         <v>28</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>9</v>
       </c>
-      <c r="H72">
+      <c r="I72">
         <v>170</v>
       </c>
-      <c r="I72">
+      <c r="J72">
         <v>34.799999999999997</v>
       </c>
-      <c r="J72">
+      <c r="K72">
         <v>1188.5999999999999</v>
       </c>
-      <c r="K72">
+      <c r="L72">
         <v>349</v>
       </c>
-      <c r="L72">
+      <c r="M72">
         <v>0.3</v>
       </c>
-      <c r="M72">
+      <c r="N72">
         <v>2.94</v>
       </c>
-      <c r="N72">
+      <c r="O72">
         <v>118424</v>
       </c>
-      <c r="O72">
+      <c r="P72">
         <v>6193</v>
       </c>
-      <c r="P72">
+      <c r="Q72">
         <v>10</v>
       </c>
-      <c r="Q72">
+      <c r="R72">
         <v>76.3</v>
       </c>
-      <c r="R72">
+      <c r="S72">
         <v>41</v>
       </c>
-      <c r="S72">
+      <c r="T72">
         <v>0</v>
       </c>
-      <c r="T72">
+      <c r="U72">
         <v>0.13</v>
       </c>
-      <c r="U72">
+      <c r="V72">
         <v>12740</v>
       </c>
-      <c r="V72">
+      <c r="W72">
         <v>1086</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>57</v>
       </c>
       <c r="B73" t="s">
-        <v>30</v>
-      </c>
-      <c r="C73">
+        <v>58</v>
+      </c>
+      <c r="C73" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73">
         <v>4</v>
       </c>
-      <c r="D73" s="1">
+      <c r="E73" s="1">
         <v>41772</v>
       </c>
-      <c r="E73" s="1">
+      <c r="F73" s="1">
         <v>41954</v>
       </c>
-      <c r="F73" t="s">
+      <c r="G73" t="s">
         <v>25</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>9</v>
       </c>
-      <c r="H73">
+      <c r="I73">
         <v>182</v>
       </c>
-      <c r="I73">
+      <c r="J73">
         <v>26.7</v>
       </c>
-      <c r="J73">
+      <c r="K73">
         <v>721.9</v>
       </c>
-      <c r="K73">
+      <c r="L73">
         <v>137.6</v>
       </c>
-      <c r="L73">
+      <c r="M73">
         <v>0.2</v>
       </c>
-      <c r="M73">
+      <c r="N73">
         <v>3.32</v>
       </c>
-      <c r="N73">
+      <c r="O73">
         <v>41315</v>
       </c>
-      <c r="O73">
+      <c r="P73">
         <v>2008</v>
       </c>
-      <c r="P73">
+      <c r="Q73">
         <v>4.7</v>
       </c>
-      <c r="Q73">
+      <c r="R73">
         <v>64.900000000000006</v>
       </c>
-      <c r="R73">
+      <c r="S73">
         <v>14.8</v>
       </c>
-      <c r="S73">
+      <c r="T73">
         <v>0</v>
       </c>
-      <c r="T73">
+      <c r="U73">
         <v>0.06</v>
       </c>
-      <c r="U73">
+      <c r="V73">
         <v>3716</v>
       </c>
-      <c r="V73">
+      <c r="W73">
         <v>212</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update observed files and improved phenology parameters in apsimx file
</commit_message>
<xml_diff>
--- a/Prototypes/Canola/Greenethorpe2014.xlsx
+++ b/Prototypes/Canola/Greenethorpe2014.xlsx
@@ -8,19 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil026\ApsimX\Prototypes\Canola\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC12D7E-2DFB-47E2-921F-129C7F040939}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AB2A52-02E1-4C2F-9658-4DC6948850B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="7590" windowWidth="31770" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3375" yWindow="3375" windowWidth="15840" windowHeight="13095" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
+    <sheet name="OBSPhenology" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$W$73</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="74">
   <si>
     <t>SimulationName</t>
   </si>
@@ -200,6 +215,48 @@
   </si>
   <si>
     <t>site</t>
+  </si>
+  <si>
+    <t>Canola.Phenology.StartFloweringDAS</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>TOS</t>
+  </si>
+  <si>
+    <t>TOS_Date</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>1-Apr</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>16-Apr</t>
+  </si>
+  <si>
+    <t>28-Apr</t>
+  </si>
+  <si>
+    <t>13-May</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Canola.Phenology.CurrentStageName</t>
+  </si>
+  <si>
+    <t>HarvestRipe</t>
   </si>
 </sst>
 </file>
@@ -1041,10 +1098,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1183,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1163,7 +1221,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1195,7 +1253,7 @@
         <v>51.1</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1233,7 +1291,7 @@
         <v>219.9</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1271,7 +1329,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1312,7 +1370,7 @@
         <v>67.2</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1383,7 +1441,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1415,7 +1473,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1453,7 +1511,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1491,7 +1549,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1529,7 +1587,7 @@
         <v>64.5</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1570,7 +1628,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -4612,6 +4670,1036 @@
       </c>
       <c r="W73">
         <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:W73" xr:uid="{724E0034-B98F-4FAB-96ED-47A4F16C5823}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="_Ex3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850B995B-358C-416B-A116-CC286325F030}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>D2&amp;E2&amp;"_Ex3Cv"&amp;B2&amp;"TOS"&amp;G2</f>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>106</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2">
+        <v>2014</v>
+      </c>
+      <c r="F2" s="1">
+        <v>41836</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>41730</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>D3&amp;E3&amp;"_Ex3Cv"&amp;B3&amp;"TOS"&amp;G3</f>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>106</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3">
+        <v>2014</v>
+      </c>
+      <c r="F3" s="1">
+        <v>41836</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>41730</v>
+      </c>
+      <c r="I3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A25" si="0">D4&amp;E4&amp;"_Ex3Cv"&amp;B4&amp;"TOS"&amp;G4</f>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4">
+        <v>2014</v>
+      </c>
+      <c r="F4" s="1">
+        <v>41816</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>41730</v>
+      </c>
+      <c r="I4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>106</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5">
+        <v>2014</v>
+      </c>
+      <c r="F5" s="1">
+        <v>41836</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <v>41730</v>
+      </c>
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6">
+        <v>2014</v>
+      </c>
+      <c r="F6" s="1">
+        <v>41807</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>41730</v>
+      </c>
+      <c r="I6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>176</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7">
+        <v>2014</v>
+      </c>
+      <c r="F7" s="1">
+        <v>41906</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>41730</v>
+      </c>
+      <c r="I7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>112</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8">
+        <v>2014</v>
+      </c>
+      <c r="F8" s="1">
+        <v>41857</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1">
+        <v>41745</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8">
+        <v>16</v>
+      </c>
+      <c r="K8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>112</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9">
+        <v>2014</v>
+      </c>
+      <c r="F9" s="1">
+        <v>41857</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>41745</v>
+      </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9">
+        <v>16</v>
+      </c>
+      <c r="K9" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>105</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10">
+        <v>2014</v>
+      </c>
+      <c r="F10" s="1">
+        <v>41850</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1">
+        <v>41745</v>
+      </c>
+      <c r="I10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10">
+        <v>16</v>
+      </c>
+      <c r="K10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11">
+        <v>112</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11">
+        <v>2014</v>
+      </c>
+      <c r="F11" s="1">
+        <v>41857</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>41745</v>
+      </c>
+      <c r="I11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11">
+        <v>16</v>
+      </c>
+      <c r="K11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>105</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12">
+        <v>2014</v>
+      </c>
+      <c r="F12" s="1">
+        <v>41850</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1">
+        <v>41745</v>
+      </c>
+      <c r="I12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>161</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13">
+        <v>2014</v>
+      </c>
+      <c r="F13" s="1">
+        <v>41906</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>41745</v>
+      </c>
+      <c r="I13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13">
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>113</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14">
+        <v>2014</v>
+      </c>
+      <c r="F14" s="1">
+        <v>41870</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14" s="1">
+        <v>41757</v>
+      </c>
+      <c r="I14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14">
+        <v>28</v>
+      </c>
+      <c r="K14" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15">
+        <v>113</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15">
+        <v>2014</v>
+      </c>
+      <c r="F15" s="1">
+        <v>41870</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15" s="1">
+        <v>41757</v>
+      </c>
+      <c r="I15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15">
+        <v>28</v>
+      </c>
+      <c r="K15" t="s">
+        <v>67</v>
+      </c>
+      <c r="L15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>106</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16">
+        <v>2014</v>
+      </c>
+      <c r="F16" s="1">
+        <v>41863</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16" s="1">
+        <v>41757</v>
+      </c>
+      <c r="I16" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16">
+        <v>28</v>
+      </c>
+      <c r="K16" t="s">
+        <v>67</v>
+      </c>
+      <c r="L16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <v>113</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17">
+        <v>2014</v>
+      </c>
+      <c r="F17" s="1">
+        <v>41870</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1">
+        <v>41757</v>
+      </c>
+      <c r="I17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17">
+        <v>28</v>
+      </c>
+      <c r="K17" t="s">
+        <v>67</v>
+      </c>
+      <c r="L17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>106</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18">
+        <v>2014</v>
+      </c>
+      <c r="F18" s="1">
+        <v>41863</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18" s="1">
+        <v>41757</v>
+      </c>
+      <c r="I18" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18">
+        <v>28</v>
+      </c>
+      <c r="K18" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>155</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19">
+        <v>2014</v>
+      </c>
+      <c r="F19" s="1">
+        <v>41912</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19" s="1">
+        <v>41757</v>
+      </c>
+      <c r="I19" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19">
+        <v>28</v>
+      </c>
+      <c r="K19" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3Cv44Y87_CLTOS4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <v>113</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20">
+        <v>2014</v>
+      </c>
+      <c r="F20" s="1">
+        <v>41885</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20" s="1">
+        <v>41772</v>
+      </c>
+      <c r="I20" t="s">
+        <v>70</v>
+      </c>
+      <c r="J20">
+        <v>13</v>
+      </c>
+      <c r="K20" t="s">
+        <v>71</v>
+      </c>
+      <c r="L20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3Cv45Y88_CLTOS4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21">
+        <v>113</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21">
+        <v>2014</v>
+      </c>
+      <c r="F21" s="1">
+        <v>41885</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21" s="1">
+        <v>41772</v>
+      </c>
+      <c r="I21" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21">
+        <v>13</v>
+      </c>
+      <c r="K21" t="s">
+        <v>71</v>
+      </c>
+      <c r="L21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvATR_GemTOS4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22">
+        <v>113</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22">
+        <v>2014</v>
+      </c>
+      <c r="F22" s="1">
+        <v>41885</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22" s="1">
+        <v>41772</v>
+      </c>
+      <c r="I22" t="s">
+        <v>70</v>
+      </c>
+      <c r="J22">
+        <v>13</v>
+      </c>
+      <c r="K22" t="s">
+        <v>71</v>
+      </c>
+      <c r="L22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola559_TTTOS4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23">
+        <v>113</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23">
+        <v>2014</v>
+      </c>
+      <c r="F23" s="1">
+        <v>41885</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23" s="1">
+        <v>41772</v>
+      </c>
+      <c r="I23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23">
+        <v>13</v>
+      </c>
+      <c r="K23" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola575_CLTOS4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24">
+        <v>113</v>
+      </c>
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24">
+        <v>2014</v>
+      </c>
+      <c r="F24" s="1">
+        <v>41885</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24" s="1">
+        <v>41772</v>
+      </c>
+      <c r="I24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J24">
+        <v>13</v>
+      </c>
+      <c r="K24" t="s">
+        <v>71</v>
+      </c>
+      <c r="L24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>Greenethorpe2014_Ex3CvHyola971_CLTOS4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>147</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25">
+        <v>2014</v>
+      </c>
+      <c r="F25" s="1">
+        <v>41919</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25" s="1">
+        <v>41772</v>
+      </c>
+      <c r="I25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25">
+        <v>13</v>
+      </c>
+      <c r="K25" t="s">
+        <v>71</v>
+      </c>
+      <c r="L25" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>